<commit_message>
Skills now have types.
We can use these types to get the right skill when filtering.
Fixed Tests.
</commit_message>
<xml_diff>
--- a/resources/data-imports/kingdoms.xlsx
+++ b/resources/data-imports/kingdoms.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
   <si>
     <t>name</t>
   </si>
@@ -103,6 +103,66 @@
     <t>increase_defence_amount</t>
   </si>
   <si>
+    <t>Keep</t>
+  </si>
+  <si>
+    <t>This is where you live. There is nothing special about this building, accept if it falls your kingdom looses 15% morale per hour.</t>
+  </si>
+  <si>
+    <t>Farm</t>
+  </si>
+  <si>
+    <t>This is how you feed your population and grow your population. The higher the level the more population gain per hour as well as overall. Should this building fall your kingdom will lose 5% morale per hour. People don't like to starve.</t>
+  </si>
+  <si>
+    <t>Lumber Mill</t>
+  </si>
+  <si>
+    <t>This is how your kingdom gets wood. Wood is useful for buildings and units.</t>
+  </si>
+  <si>
+    <t>Stone Quarry</t>
+  </si>
+  <si>
+    <t>This is how your kingdom gets stone. Stone is used for some units, but mostly buildings.</t>
+  </si>
+  <si>
+    <t>Clay Pit</t>
+  </si>
+  <si>
+    <t>This is how your kingdom gets clay. Clay is used in buildings and for some units.</t>
+  </si>
+  <si>
+    <t>Iron Mine</t>
+  </si>
+  <si>
+    <t>This is how your kingdom gets iron. Iron is used for both units and buildings.</t>
+  </si>
+  <si>
+    <t>Walls</t>
+  </si>
+  <si>
+    <t>This is how your kingdom is protected, walls are important. Siege weapons have a harder time trampling over your kingdoms if the walls are higher in level they will give a bonus to defence of the kingdom. Should this building fall, your kingdom will lose 10% morale per hour. People don't like to live in kingdoms without walls.</t>
+  </si>
+  <si>
+    <t>Barracks</t>
+  </si>
+  <si>
+    <t>This is where you recruit units. The higher the level, the more unit types you can recruit. Should this building fall, your kingdom will lose 8% morale per hour. People do not like to live in a kingdom where their king cannot protect them.</t>
+  </si>
+  <si>
+    <t>Church</t>
+  </si>
+  <si>
+    <t>This is where your people pray and, as the building levels, where you can recruit special healers and units who can both attack and heal as well as defend and heal. Should this building fall, your kingdom will lose 5% morale per hour. Your people need a place to feel safe.</t>
+  </si>
+  <si>
+    <t>Settlers Hall</t>
+  </si>
+  <si>
+    <t>This is how you get settler units, starting at level 10, to be able to settle other kingdoms and take them over. Never send a settler alone. Sending more the one in the same attack (from the same kingdom) will not stack the morale deduction these special units do to a kingdom.</t>
+  </si>
+  <si>
     <t>attack</t>
   </si>
   <si>
@@ -149,6 +209,63 @@
   </si>
   <si>
     <t>time_to_recruit</t>
+  </si>
+  <si>
+    <t>Spearmen</t>
+  </si>
+  <si>
+    <t>These units are weak, but good for defending with their one and only weapon: The spear. They move quick, take little time to recruit and use little resources.</t>
+  </si>
+  <si>
+    <t>Archer</t>
+  </si>
+  <si>
+    <t>Archers are a good unit to have, they are the best attackers and defenders. They move quick and use little resources.</t>
+  </si>
+  <si>
+    <t>Swordsmen</t>
+  </si>
+  <si>
+    <t>These units are well armoured and well trained. The best of the best for defenders and attacking. They require a bit more resources, move a tad slower, but they're attack is well aimed.</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Slow moving unit that will attack walls and then farms. These are the best units for taking down walls next to Trebuchets. Not very good for defending but great for attacking.</t>
+  </si>
+  <si>
+    <t>Trebuchet</t>
+  </si>
+  <si>
+    <t>These are the best units for siege units. They can obliterate walls, buildings and when used as defenders - even enemies. Any kingdom with these units is a kingdom to be feared.</t>
+  </si>
+  <si>
+    <t>Buildings</t>
+  </si>
+  <si>
+    <t>Priest</t>
+  </si>
+  <si>
+    <t>This unit does not attack or defend, but heals. Should you send more then one, the healing will stack.</t>
+  </si>
+  <si>
+    <t>Cleric</t>
+  </si>
+  <si>
+    <t>These units can not only heal but attack and defend your kingdom. Sending multiple, the healing will stack.</t>
+  </si>
+  <si>
+    <t>Paladin</t>
+  </si>
+  <si>
+    <t>These units have a higher healing rate and are great for defenders and attacking. They move slower, but their healing stacks with the more sent.</t>
+  </si>
+  <si>
+    <t>Settler</t>
+  </si>
+  <si>
+    <t>This unit will reduce the morale by 10% when sent to a kingdom. Never send this unit alone, for they will stumble over a rock and die. When they arrive at the kingdom and reduce the kingdoms morale, they will die - if they do not take the kingdom. If they do, they will become apart of your kingdom. They cannot attack or defend. You must send them with regular units, not siege units or healing based units.</t>
   </si>
   <si>
     <t>Building Name</t>
@@ -496,7 +613,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:AB11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,8 +621,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="388" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="11" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="18" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="15" bestFit="true" customWidth="true" style="0"/>
@@ -620,6 +737,698 @@
         <v>27</v>
       </c>
     </row>
+    <row r="2" spans="1:28">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>250</v>
+      </c>
+      <c r="E2">
+        <v>250</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>100</v>
+      </c>
+      <c r="O2">
+        <v>50</v>
+      </c>
+      <c r="P2">
+        <v>125</v>
+      </c>
+      <c r="Q2">
+        <v>75</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0.15</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0.05</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>70</v>
+      </c>
+      <c r="AB2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>75</v>
+      </c>
+      <c r="E3">
+        <v>75</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>75</v>
+      </c>
+      <c r="O3">
+        <v>50</v>
+      </c>
+      <c r="P3">
+        <v>75</v>
+      </c>
+      <c r="Q3">
+        <v>25</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0.05</v>
+      </c>
+      <c r="U3">
+        <v>100</v>
+      </c>
+      <c r="V3">
+        <v>0.03</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>35</v>
+      </c>
+      <c r="AB3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>65</v>
+      </c>
+      <c r="E4">
+        <v>65</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>50</v>
+      </c>
+      <c r="O4">
+        <v>25</v>
+      </c>
+      <c r="P4">
+        <v>50</v>
+      </c>
+      <c r="Q4">
+        <v>45</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>100</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>25</v>
+      </c>
+      <c r="AB4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>55</v>
+      </c>
+      <c r="E5">
+        <v>75</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>75</v>
+      </c>
+      <c r="O5">
+        <v>25</v>
+      </c>
+      <c r="P5">
+        <v>40</v>
+      </c>
+      <c r="Q5">
+        <v>75</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>85</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>25</v>
+      </c>
+      <c r="AB5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>50</v>
+      </c>
+      <c r="O6">
+        <v>20</v>
+      </c>
+      <c r="P6">
+        <v>25</v>
+      </c>
+      <c r="Q6">
+        <v>30</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>110</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>25</v>
+      </c>
+      <c r="AB6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>80</v>
+      </c>
+      <c r="E7">
+        <v>75</v>
+      </c>
+      <c r="F7">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>80</v>
+      </c>
+      <c r="O7">
+        <v>30</v>
+      </c>
+      <c r="P7">
+        <v>40</v>
+      </c>
+      <c r="Q7">
+        <v>80</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>80</v>
+      </c>
+      <c r="AA7">
+        <v>20</v>
+      </c>
+      <c r="AB7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>150</v>
+      </c>
+      <c r="E8">
+        <v>150</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>100</v>
+      </c>
+      <c r="O8">
+        <v>70</v>
+      </c>
+      <c r="P8">
+        <v>200</v>
+      </c>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0.1</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0.05</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>75</v>
+      </c>
+      <c r="AB8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9">
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9">
+        <v>80</v>
+      </c>
+      <c r="F9">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>90</v>
+      </c>
+      <c r="O9">
+        <v>45</v>
+      </c>
+      <c r="P9">
+        <v>100</v>
+      </c>
+      <c r="Q9">
+        <v>100</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0.08</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0.04</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>60</v>
+      </c>
+      <c r="AB9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>75</v>
+      </c>
+      <c r="E10">
+        <v>75</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>100</v>
+      </c>
+      <c r="O10">
+        <v>50</v>
+      </c>
+      <c r="P10">
+        <v>120</v>
+      </c>
+      <c r="Q10">
+        <v>75</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0.05</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0.05</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>30</v>
+      </c>
+      <c r="AB10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>70</v>
+      </c>
+      <c r="E11">
+        <v>70</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>100</v>
+      </c>
+      <c r="O11">
+        <v>100</v>
+      </c>
+      <c r="P11">
+        <v>100</v>
+      </c>
+      <c r="Q11">
+        <v>100</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>40</v>
+      </c>
+      <c r="AB11">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
@@ -641,7 +1450,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,8 +1458,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="482" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="8" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="21" bestFit="true" customWidth="true" style="0"/>
@@ -682,49 +1491,49 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="K1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="M1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="N1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="O1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="P1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="Q1" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="R1" t="s">
         <v>13</v>
@@ -742,7 +1551,448 @@
         <v>5</v>
       </c>
       <c r="W1" t="s">
-        <v>43</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>5</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>5</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>10</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <v>25</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>15</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="W5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>70</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>25</v>
+      </c>
+      <c r="U6">
+        <v>25</v>
+      </c>
+      <c r="V6">
+        <v>5</v>
+      </c>
+      <c r="W6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0.003</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>5</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0.005</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>8</v>
+      </c>
+      <c r="S8">
+        <v>5</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>6</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0.01</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>8</v>
+      </c>
+      <c r="S9">
+        <v>8</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>10</v>
+      </c>
+      <c r="V9">
+        <v>2</v>
+      </c>
+      <c r="W9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>20</v>
+      </c>
+      <c r="R10">
+        <v>200</v>
+      </c>
+      <c r="S10">
+        <v>200</v>
+      </c>
+      <c r="T10">
+        <v>200</v>
+      </c>
+      <c r="U10">
+        <v>200</v>
+      </c>
+      <c r="V10">
+        <v>50</v>
+      </c>
+      <c r="W10">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +2016,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -781,13 +2031,112 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes, documentation changes and various little tweaks
</commit_message>
<xml_diff>
--- a/resources/data-imports/kingdoms.xlsx
+++ b/resources/data-imports/kingdoms.xlsx
@@ -1,39 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817E675B-CA92-8148-A9A6-7C594746951F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Buildings" sheetId="1" r:id="rId1"/>
-    <sheet name="Units" sheetId="2" r:id="rId2"/>
-    <sheet name="Building Units" sheetId="3" r:id="rId3"/>
+    <sheet name="Buildings" sheetId="1" r:id="rId4"/>
+    <sheet name="Units" sheetId="2" r:id="rId5"/>
+    <sheet name="Building Units" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" forceFullCalc="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
     <t>name</t>
   </si>
@@ -341,9 +325,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -354,37 +343,28 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -674,47 +654,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:AE14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="388" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="31" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="24" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="25" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="31" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="388" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="31" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="25" max="25" width="25" bestFit="true" customWidth="true" style="0"/>
+    <col min="26" max="26" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="27" max="27" width="31" bestFit="true" customWidth="true" style="0"/>
+    <col min="28" max="28" width="28" bestFit="true" customWidth="true" style="0"/>
+    <col min="29" max="29" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="30" max="30" width="29" bestFit="true" customWidth="true" style="0"/>
+    <col min="31" max="31" width="17" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +794,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -874,7 +859,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -942,7 +927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1010,7 +995,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1078,7 +1063,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1146,7 +1131,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1214,7 +1199,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1282,7 +1267,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1353,7 +1338,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1427,7 +1412,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1501,7 +1486,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1575,7 +1560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1658,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1739,44 +1724,60 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="482" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="482" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="8" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="17" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="18" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1891,7 +1892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1938,7 +1939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -1985,7 +1986,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -2035,7 +2036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -2088,7 +2089,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -2105,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>3.0000000000000001E-3</v>
+        <v>0.003</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -2135,7 +2136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -2152,7 +2153,7 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -2188,7 +2189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -2241,7 +2242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -2288,7 +2289,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -2341,7 +2342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
         <v>94</v>
       </c>
@@ -2385,7 +2386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -2427,26 +2428,40 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="17" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -2457,7 +2472,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2468,7 +2483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -2479,7 +2494,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -2490,7 +2505,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -2501,7 +2516,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -2512,7 +2527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -2523,7 +2538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -2534,7 +2549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -2545,7 +2560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -2556,7 +2571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -2567,9 +2582,40 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed most imports to search by id instead of name.
This allows people to change the names of items with out having to go
through the admin pannel, they can just update the excell file.
</commit_message>
<xml_diff>
--- a/resources/data-imports/kingdoms.xlsx
+++ b/resources/data-imports/kingdoms.xlsx
@@ -17,7 +17,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>name</t>
   </si>
@@ -343,10 +346,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -658,7 +658,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AE14"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,40 +666,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="388" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="10" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="3" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="29" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="388" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="9" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="26" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="31" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="26" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="31" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="26" bestFit="true" customWidth="true" style="0"/>
     <col min="24" max="24" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="25" max="25" width="25" bestFit="true" customWidth="true" style="0"/>
-    <col min="26" max="26" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="27" max="27" width="31" bestFit="true" customWidth="true" style="0"/>
-    <col min="28" max="28" width="28" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="30" max="30" width="29" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="17" bestFit="true" customWidth="true" style="0"/>
+    <col min="25" max="25" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="26" max="26" width="25" bestFit="true" customWidth="true" style="0"/>
+    <col min="27" max="27" width="24" bestFit="true" customWidth="true" style="0"/>
+    <col min="28" max="28" width="31" bestFit="true" customWidth="true" style="0"/>
+    <col min="29" max="29" width="28" bestFit="true" customWidth="true" style="0"/>
+    <col min="30" max="30" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="31" max="31" width="19" bestFit="true" customWidth="true" style="0"/>
+    <col min="32" max="32" width="17" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:32">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -793,56 +794,59 @@
       <c r="AE1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:31">
-      <c r="A2" t="s">
+      <c r="AF1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2">
         <v>30</v>
-      </c>
-      <c r="D2">
-        <v>250</v>
       </c>
       <c r="E2">
         <v>250</v>
       </c>
       <c r="F2">
+        <v>250</v>
+      </c>
+      <c r="G2">
         <v>10</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>100</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>50</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>125</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>75</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>10</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>0.2</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>0.15</v>
       </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
       <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
         <v>0.05</v>
       </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
       <c r="X2">
         <v>0</v>
       </c>
@@ -853,64 +857,67 @@
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="AB2">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:31">
-      <c r="A3" t="s">
-        <v>33</v>
+      <c r="AC2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
         <v>35</v>
       </c>
       <c r="D3">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="E3">
         <v>75</v>
       </c>
       <c r="F3">
+        <v>75</v>
+      </c>
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
       <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
         <v>75</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>50</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>75</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>25</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>5</v>
-      </c>
-      <c r="S3">
-        <v>0.05</v>
       </c>
       <c r="T3">
         <v>0.05</v>
       </c>
       <c r="U3">
+        <v>0.05</v>
+      </c>
+      <c r="V3">
         <v>100</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>0.03</v>
       </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
       <c r="X3">
         <v>0</v>
       </c>
@@ -921,55 +928,58 @@
         <v>0</v>
       </c>
       <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
         <v>35</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
-      <c r="A4" t="s">
-        <v>35</v>
+    <row r="4" spans="1:32">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4">
         <v>30</v>
-      </c>
-      <c r="D4">
-        <v>65</v>
       </c>
       <c r="E4">
         <v>65</v>
       </c>
       <c r="F4">
+        <v>65</v>
+      </c>
+      <c r="G4">
         <v>10</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="N4">
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>50</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>25</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>50</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>45</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>6</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>0.08</v>
       </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
       <c r="U4">
         <v>0</v>
       </c>
@@ -977,11 +987,11 @@
         <v>0</v>
       </c>
       <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
         <v>100</v>
       </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
       <c r="Y4">
         <v>0</v>
       </c>
@@ -989,55 +999,58 @@
         <v>0</v>
       </c>
       <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
         <v>25</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
-      <c r="A5" t="s">
-        <v>37</v>
+    <row r="5" spans="1:32">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5">
         <v>30</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>55</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>75</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>15</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="N5">
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="O5">
         <v>75</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>25</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>40</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>75</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>8</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>0.1</v>
       </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
       <c r="U5">
         <v>0</v>
       </c>
@@ -1051,61 +1064,64 @@
         <v>0</v>
       </c>
       <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
         <v>85</v>
       </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
       <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
         <v>25</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
-      <c r="A6" t="s">
-        <v>39</v>
+    <row r="6" spans="1:32">
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6">
         <v>30</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>45</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>30</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>8</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="N6">
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="O6">
         <v>50</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>20</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>25</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>30</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>4</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>0.05</v>
       </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
       <c r="U6">
         <v>0</v>
       </c>
@@ -1116,64 +1132,67 @@
         <v>0</v>
       </c>
       <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
         <v>110</v>
       </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
       <c r="Z6">
         <v>0</v>
       </c>
       <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
         <v>25</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
-      <c r="A7" t="s">
-        <v>41</v>
+    <row r="7" spans="1:32">
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7">
         <v>30</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>80</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>75</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>18</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="N7">
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="O7">
         <v>80</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>30</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>40</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>80</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>9</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>0.12</v>
       </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
       <c r="U7">
         <v>0</v>
       </c>
@@ -1190,67 +1209,70 @@
         <v>0</v>
       </c>
       <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
         <v>80</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <v>20</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
-      <c r="A8" t="s">
-        <v>43</v>
+    <row r="8" spans="1:32">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8">
         <v>30</v>
-      </c>
-      <c r="D8">
-        <v>150</v>
       </c>
       <c r="E8">
         <v>150</v>
       </c>
       <c r="F8">
+        <v>150</v>
+      </c>
+      <c r="G8">
         <v>20</v>
       </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="N8">
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="O8">
         <v>100</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>70</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>200</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>100</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>12</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>0.15</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>0.1</v>
       </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
       <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
         <v>0.05</v>
       </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
       <c r="X8">
         <v>0</v>
       </c>
@@ -1261,67 +1283,70 @@
         <v>0</v>
       </c>
       <c r="AA8">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="AB8">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:31">
-      <c r="A9" t="s">
-        <v>45</v>
+      <c r="AC8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32">
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>46</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9">
         <v>35</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>100</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>80</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>15</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>5</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="N9">
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="O9">
         <v>90</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>45</v>
-      </c>
-      <c r="P9">
-        <v>100</v>
       </c>
       <c r="Q9">
         <v>100</v>
       </c>
       <c r="R9">
+        <v>100</v>
+      </c>
+      <c r="S9">
         <v>7</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>0.13</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>0.08</v>
       </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
       <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
         <v>0.04</v>
       </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
       <c r="X9">
         <v>0</v>
       </c>
@@ -1332,70 +1357,73 @@
         <v>0</v>
       </c>
       <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
         <v>60</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
-      <c r="A10" t="s">
-        <v>47</v>
+    <row r="10" spans="1:32">
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10">
         <v>12</v>
-      </c>
-      <c r="D10">
-        <v>75</v>
       </c>
       <c r="E10">
         <v>75</v>
       </c>
       <c r="F10">
+        <v>75</v>
+      </c>
+      <c r="G10">
         <v>9</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>3</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="N10">
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="O10">
         <v>100</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>50</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>120</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>75</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>11</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>0.16</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>0.05</v>
       </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
       <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
         <v>0.05</v>
       </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
       <c r="X10">
         <v>0</v>
       </c>
@@ -1406,42 +1434,45 @@
         <v>0</v>
       </c>
       <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
         <v>30</v>
       </c>
-      <c r="AB10">
+      <c r="AC10">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
-      <c r="A11" t="s">
-        <v>49</v>
+    <row r="11" spans="1:32">
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11">
         <v>20</v>
-      </c>
-      <c r="D11">
-        <v>70</v>
       </c>
       <c r="E11">
         <v>70</v>
       </c>
       <c r="F11">
+        <v>70</v>
+      </c>
+      <c r="G11">
         <v>20</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
       <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <v>10</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>100</v>
+      <c r="K11">
+        <v>1</v>
       </c>
       <c r="O11">
         <v>100</v>
@@ -1453,14 +1484,14 @@
         <v>100</v>
       </c>
       <c r="R11">
+        <v>100</v>
+      </c>
+      <c r="S11">
         <v>15</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>0.25</v>
       </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
       <c r="U11">
         <v>0</v>
       </c>
@@ -1480,52 +1511,55 @@
         <v>0</v>
       </c>
       <c r="AA11">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AB11">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:31">
-      <c r="A12" t="s">
-        <v>51</v>
+      <c r="AC11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32">
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12">
         <v>10</v>
-      </c>
-      <c r="D12">
-        <v>150</v>
       </c>
       <c r="E12">
         <v>150</v>
       </c>
       <c r="F12">
+        <v>150</v>
+      </c>
+      <c r="G12">
         <v>100</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>100</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>250</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>500</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>700</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>14</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>0.18</v>
       </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
       <c r="U12">
         <v>0</v>
       </c>
@@ -1545,70 +1579,73 @@
         <v>0</v>
       </c>
       <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
         <v>75</v>
       </c>
-      <c r="AB12">
+      <c r="AC12">
         <v>112</v>
       </c>
-      <c r="AC12">
-        <v>1</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>51</v>
+      <c r="AD12">
+        <v>1</v>
       </c>
       <c r="AE12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31">
-      <c r="A13" t="s">
-        <v>53</v>
+        <v>5</v>
+      </c>
+      <c r="AF12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32">
+      <c r="A13">
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>54</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13">
         <v>20</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>200</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>150</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>100</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
       <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
         <v>10</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>200</v>
+      <c r="K13">
+        <v>1</v>
       </c>
       <c r="O13">
         <v>200</v>
       </c>
       <c r="P13">
+        <v>200</v>
+      </c>
+      <c r="Q13">
         <v>300</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>1000</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>18</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>0.19</v>
       </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
       <c r="U13">
         <v>0</v>
       </c>
@@ -1628,67 +1665,70 @@
         <v>0</v>
       </c>
       <c r="AA13">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AB13">
         <v>50</v>
       </c>
       <c r="AC13">
-        <v>1</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="AD13">
+        <v>1</v>
       </c>
       <c r="AE13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31">
-      <c r="A14" t="s">
-        <v>55</v>
+        <v>7</v>
+      </c>
+      <c r="AF13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32">
+      <c r="A14">
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14">
         <v>20</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>150</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>175</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>100</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>5</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="N14">
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="O14">
         <v>150</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>75</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>200</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>300</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>10</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>0.12</v>
       </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
       <c r="U14">
         <v>0</v>
       </c>
@@ -1708,18 +1748,21 @@
         <v>0</v>
       </c>
       <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
         <v>50</v>
       </c>
-      <c r="AB14">
+      <c r="AC14">
         <v>60</v>
       </c>
-      <c r="AC14">
-        <v>1</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>55</v>
+      <c r="AD14">
+        <v>1</v>
       </c>
       <c r="AE14">
+        <v>9</v>
+      </c>
+      <c r="AF14">
         <v>1</v>
       </c>
     </row>
@@ -1744,7 +1787,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1752,32 +1795,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="482" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="10" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="3" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="482" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="8" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="21" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="10" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="17" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="18" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1785,7 +1829,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>58</v>
@@ -1830,7 +1874,7 @@
         <v>71</v>
       </c>
       <c r="R1" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="S1" t="s">
         <v>14</v>
@@ -1842,436 +1886,463 @@
         <v>16</v>
       </c>
       <c r="V1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="W1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
-      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="X1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>74</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>75</v>
       </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>1</v>
       </c>
       <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
         <v>5</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
       <c r="T2">
         <v>0</v>
       </c>
       <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
         <v>2</v>
       </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
       <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
-      <c r="A3" t="s">
-        <v>75</v>
+    <row r="3" spans="1:24">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>76</v>
       </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="C3" t="s">
+        <v>77</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="K3">
-        <v>0</v>
+      <c r="E3">
+        <v>2</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
-      <c r="Q3">
+      <c r="O3">
         <v>1</v>
       </c>
       <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
         <v>5</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
       <c r="T3">
         <v>0</v>
       </c>
       <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
         <v>5</v>
       </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
       <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
-      <c r="A4" t="s">
-        <v>77</v>
+    <row r="4" spans="1:24">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>78</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
-      <c r="Q4">
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="R4">
         <v>2</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>5</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
       <c r="T4">
         <v>0</v>
       </c>
       <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
         <v>10</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>2</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
-      <c r="A5" t="s">
-        <v>79</v>
+    <row r="5" spans="1:24">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>80</v>
       </c>
-      <c r="C5">
-        <v>5</v>
+      <c r="C5" t="s">
+        <v>81</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
-      <c r="J5">
-        <v>1</v>
+      <c r="E5">
+        <v>5</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="O5" t="s">
-        <v>43</v>
+      <c r="M5">
+        <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q5">
+        <v>44</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5">
         <v>3</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>25</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
       <c r="T5">
         <v>0</v>
       </c>
       <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
         <v>15</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>3</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
-      <c r="A6" t="s">
-        <v>81</v>
+    <row r="6" spans="1:24">
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>82</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6">
         <v>10</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>6</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="O6" t="s">
-        <v>43</v>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q6">
+        <v>44</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>84</v>
+      </c>
+      <c r="R6">
         <v>5</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>70</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
       <c r="T6">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="U6">
         <v>25</v>
       </c>
       <c r="V6">
+        <v>25</v>
+      </c>
+      <c r="W6">
         <v>5</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
-      <c r="A7" t="s">
-        <v>84</v>
+    <row r="7" spans="1:24">
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>85</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" t="s">
+        <v>86</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="H7">
-        <v>1</v>
+      <c r="E7">
+        <v>0</v>
       </c>
       <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
         <v>0.003</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
       <c r="L7">
         <v>0</v>
       </c>
-      <c r="Q7">
-        <v>1</v>
+      <c r="M7">
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
         <v>5</v>
       </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
       <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
         <v>5</v>
       </c>
-      <c r="V7">
-        <v>1</v>
-      </c>
       <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
-      <c r="A8" t="s">
-        <v>86</v>
+    <row r="8" spans="1:24">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>87</v>
       </c>
-      <c r="C8">
-        <v>2</v>
+      <c r="C8" t="s">
+        <v>88</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
-      <c r="H8">
-        <v>1</v>
+      <c r="E8">
+        <v>2</v>
       </c>
       <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
         <v>0.005</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <v>1</v>
       </c>
-      <c r="Q8">
+      <c r="O8">
         <v>1</v>
       </c>
       <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
         <v>8</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>5</v>
       </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
       <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
         <v>6</v>
       </c>
-      <c r="V8">
-        <v>1</v>
-      </c>
       <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
-      <c r="A9" t="s">
-        <v>88</v>
+    <row r="9" spans="1:24">
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>89</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9">
         <v>3</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>4</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
       <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
         <v>0.01</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
         <v>1</v>
       </c>
-      <c r="Q9">
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="R9">
         <v>3</v>
-      </c>
-      <c r="R9">
-        <v>8</v>
       </c>
       <c r="S9">
         <v>8</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
         <v>10</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>2</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
-      <c r="A10" t="s">
-        <v>90</v>
+    <row r="10" spans="1:24">
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>91</v>
       </c>
-      <c r="C10">
-        <v>0</v>
+      <c r="C10" t="s">
+        <v>92</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>1</v>
+      <c r="E10">
+        <v>0</v>
       </c>
       <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>0.1</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="Q10">
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="R10">
         <v>20</v>
-      </c>
-      <c r="R10">
-        <v>200</v>
       </c>
       <c r="S10">
         <v>200</v>
@@ -2283,147 +2354,159 @@
         <v>200</v>
       </c>
       <c r="V10">
+        <v>200</v>
+      </c>
+      <c r="W10">
         <v>50</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
-      <c r="A11" t="s">
-        <v>92</v>
+    <row r="11" spans="1:24">
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>93</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11">
         <v>20</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>15</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11" t="s">
-        <v>43</v>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q11">
+        <v>44</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>84</v>
+      </c>
+      <c r="R11">
         <v>8</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>10</v>
-      </c>
-      <c r="S11">
-        <v>5</v>
       </c>
       <c r="T11">
         <v>5</v>
       </c>
       <c r="U11">
+        <v>5</v>
+      </c>
+      <c r="V11">
         <v>100</v>
-      </c>
-      <c r="V11">
-        <v>15</v>
       </c>
       <c r="W11">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:23">
-      <c r="A12" t="s">
-        <v>94</v>
+      <c r="X11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>95</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12">
         <v>3</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>8</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="N12">
         <v>1</v>
       </c>
       <c r="R12">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="S12">
         <v>25</v>
       </c>
       <c r="T12">
+        <v>25</v>
+      </c>
+      <c r="U12">
         <v>50</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>100</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>5</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
-      <c r="A13" t="s">
-        <v>96</v>
+    <row r="13" spans="1:24">
+      <c r="A13">
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>97</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13">
         <v>4</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>2</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
       <c r="L13">
         <v>0</v>
       </c>
-      <c r="Q13">
-        <v>1</v>
+      <c r="M13">
+        <v>0</v>
       </c>
       <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
         <v>20</v>
-      </c>
-      <c r="S13">
-        <v>25</v>
       </c>
       <c r="T13">
         <v>25</v>
       </c>
       <c r="U13">
+        <v>25</v>
+      </c>
+      <c r="V13">
         <v>50</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>5</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>6</v>
       </c>
     </row>
@@ -2448,7 +2531,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -2456,14 +2539,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="17" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="3" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="17" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>99</v>
@@ -2471,136 +2555,175 @@
       <c r="C1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
       </c>
       <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>77</v>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
       </c>
       <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>79</v>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
       </c>
       <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>81</v>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
       </c>
       <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>84</v>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" t="s">
-        <v>86</v>
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
       </c>
       <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>88</v>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
       </c>
       <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" t="s">
-        <v>90</v>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
       </c>
       <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" t="s">
-        <v>92</v>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" t="s">
-        <v>94</v>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" t="s">
-        <v>96</v>
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>33</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
       </c>
       <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
         <v>6</v>
       </c>
     </row>

</xml_diff>